<commit_message>
Added M x N dimensions
</commit_message>
<xml_diff>
--- a/Examples/Forest Fire/excel/example.xlsx
+++ b/Examples/Forest Fire/excel/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wikto\PycharmProjects\MasterDegree\Examples\Forest Fire\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wikto\Desktop\homework\MasterDegree\Examples\Forest Fire\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91996B78-7C17-43D7-8394-4545C795A2DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FF3276-9DE7-4713-AF3E-B993338D930C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="1755" windowWidth="21600" windowHeight="11835" xr2:uid="{CACAD4C5-5037-44B5-AF02-A22C5524F177}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{CACAD4C5-5037-44B5-AF02-A22C5524F177}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="3" r:id="rId1"/>
@@ -455,21 +455,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB931813-54FA-45A2-87BE-36CD6A2336B8}">
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -543,7 +548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -617,7 +622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -691,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -765,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -839,7 +844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -913,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
@@ -987,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1061,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1135,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1209,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -1283,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1357,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -1431,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -1505,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1579,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -1653,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1727,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1801,7 +1806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1875,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -1949,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2023,7 +2028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
@@ -2097,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2171,7 +2176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -2245,27 +2250,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>1</v>
       </c>
@@ -2282,19 +2287,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2368,7 +2373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2442,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2516,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2590,7 +2595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2664,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -2738,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
@@ -2812,7 +2817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -2886,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -2960,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -3034,7 +3039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -3108,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3182,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3256,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -3330,7 +3335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -3404,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -3478,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -3552,7 +3557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -3700,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -3774,7 +3779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
@@ -3848,7 +3853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
@@ -3922,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -3996,7 +4001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -4070,7 +4075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>